<commit_message>
Diubah semua ke F4
</commit_message>
<xml_diff>
--- a/buku musyrif.xlsx
+++ b/buku musyrif.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zen\buku-tahfidz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A416A1BC-EE20-4E38-B499-F9FCDD5012C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1983362B-D636-43B5-82EE-D6F577D4A82C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19890" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19890" windowHeight="8265" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kehadiran musyrif" sheetId="11" r:id="rId1"/>
@@ -817,89 +817,122 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -910,39 +943,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1229,7 +1229,7 @@
   </sheetPr>
   <dimension ref="A1:XFC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7:K7"/>
     </sheetView>
   </sheetViews>
@@ -1241,40 +1241,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="26.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="77"/>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="77"/>
-      <c r="AF1" s="77"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="92"/>
+      <c r="AA1" s="92"/>
+      <c r="AB1" s="92"/>
+      <c r="AC1" s="92"/>
+      <c r="AD1" s="92"/>
+      <c r="AE1" s="92"/>
+      <c r="AF1" s="92"/>
     </row>
     <row r="2" spans="1:32">
       <c r="H2" s="61"/>
@@ -1283,54 +1283,54 @@
       <c r="A3" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="R3" s="78"/>
-      <c r="S3" s="78"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="78" t="s">
+      <c r="B3" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
+      <c r="Q3" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" s="81"/>
+      <c r="S3" s="81"/>
+      <c r="T3" s="81"/>
+      <c r="U3" s="81"/>
+      <c r="V3" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="W3" s="78"/>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="78"/>
-      <c r="Z3" s="78"/>
-      <c r="AA3" s="78" t="s">
+      <c r="W3" s="81"/>
+      <c r="X3" s="81"/>
+      <c r="Y3" s="81"/>
+      <c r="Z3" s="81"/>
+      <c r="AA3" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="AB3" s="78"/>
-      <c r="AC3" s="78"/>
-      <c r="AD3" s="78"/>
-      <c r="AE3" s="78"/>
-      <c r="AF3" s="92" t="s">
+      <c r="AB3" s="81"/>
+      <c r="AC3" s="81"/>
+      <c r="AD3" s="81"/>
+      <c r="AE3" s="81"/>
+      <c r="AF3" s="77" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="78">
+      <c r="A4" s="81">
         <v>1</v>
       </c>
       <c r="B4" s="39">
@@ -1423,10 +1423,10 @@
       <c r="AE4" s="39">
         <v>5</v>
       </c>
-      <c r="AF4" s="92"/>
+      <c r="AF4" s="77"/>
     </row>
     <row r="5" spans="1:32" ht="18.95" customHeight="1">
-      <c r="A5" s="78"/>
+      <c r="A5" s="81"/>
       <c r="B5" s="42"/>
       <c r="C5" s="43"/>
       <c r="D5" s="43"/>
@@ -1496,54 +1496,54 @@
       <c r="A7" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="78"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="M7" s="78"/>
-      <c r="N7" s="78"/>
-      <c r="O7" s="78"/>
-      <c r="P7" s="78"/>
-      <c r="Q7" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="R7" s="78"/>
-      <c r="S7" s="78"/>
-      <c r="T7" s="78"/>
-      <c r="U7" s="78"/>
-      <c r="V7" s="78" t="s">
+      <c r="B7" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="R7" s="81"/>
+      <c r="S7" s="81"/>
+      <c r="T7" s="81"/>
+      <c r="U7" s="81"/>
+      <c r="V7" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="W7" s="78"/>
-      <c r="X7" s="78"/>
-      <c r="Y7" s="78"/>
-      <c r="Z7" s="78"/>
-      <c r="AA7" s="78" t="s">
+      <c r="W7" s="81"/>
+      <c r="X7" s="81"/>
+      <c r="Y7" s="81"/>
+      <c r="Z7" s="81"/>
+      <c r="AA7" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="AB7" s="78"/>
-      <c r="AC7" s="78"/>
-      <c r="AD7" s="78"/>
-      <c r="AE7" s="78"/>
-      <c r="AF7" s="92" t="s">
+      <c r="AB7" s="81"/>
+      <c r="AC7" s="81"/>
+      <c r="AD7" s="81"/>
+      <c r="AE7" s="81"/>
+      <c r="AF7" s="77" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:32" ht="18.95" customHeight="1">
-      <c r="A8" s="78">
+      <c r="A8" s="81">
         <v>2</v>
       </c>
       <c r="B8" s="69">
@@ -1636,10 +1636,10 @@
       <c r="AE8" s="39">
         <v>5</v>
       </c>
-      <c r="AF8" s="92"/>
+      <c r="AF8" s="77"/>
     </row>
     <row r="9" spans="1:32" ht="18.95" customHeight="1">
-      <c r="A9" s="78"/>
+      <c r="A9" s="81"/>
       <c r="B9" s="70"/>
       <c r="C9" s="43"/>
       <c r="D9" s="43"/>
@@ -1709,54 +1709,54 @@
       <c r="A11" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="78"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="M11" s="78"/>
-      <c r="N11" s="78"/>
-      <c r="O11" s="78"/>
-      <c r="P11" s="78"/>
-      <c r="Q11" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="R11" s="78"/>
-      <c r="S11" s="78"/>
-      <c r="T11" s="78"/>
-      <c r="U11" s="78"/>
-      <c r="V11" s="78" t="s">
+      <c r="B11" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" s="81"/>
+      <c r="N11" s="81"/>
+      <c r="O11" s="81"/>
+      <c r="P11" s="81"/>
+      <c r="Q11" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="R11" s="81"/>
+      <c r="S11" s="81"/>
+      <c r="T11" s="81"/>
+      <c r="U11" s="81"/>
+      <c r="V11" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="W11" s="78"/>
-      <c r="X11" s="78"/>
-      <c r="Y11" s="78"/>
-      <c r="Z11" s="78"/>
-      <c r="AA11" s="78" t="s">
+      <c r="W11" s="81"/>
+      <c r="X11" s="81"/>
+      <c r="Y11" s="81"/>
+      <c r="Z11" s="81"/>
+      <c r="AA11" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="AB11" s="78"/>
-      <c r="AC11" s="78"/>
-      <c r="AD11" s="78"/>
-      <c r="AE11" s="78"/>
-      <c r="AF11" s="92" t="s">
+      <c r="AB11" s="81"/>
+      <c r="AC11" s="81"/>
+      <c r="AD11" s="81"/>
+      <c r="AE11" s="81"/>
+      <c r="AF11" s="77" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:32" ht="18.95" customHeight="1">
-      <c r="A12" s="78">
+      <c r="A12" s="81">
         <v>3</v>
       </c>
       <c r="B12" s="39">
@@ -1849,10 +1849,10 @@
       <c r="AE12" s="39">
         <v>5</v>
       </c>
-      <c r="AF12" s="92"/>
+      <c r="AF12" s="77"/>
     </row>
     <row r="13" spans="1:32" ht="18.95" customHeight="1">
-      <c r="A13" s="78"/>
+      <c r="A13" s="81"/>
       <c r="B13" s="42"/>
       <c r="C13" s="43"/>
       <c r="D13" s="43"/>
@@ -1922,54 +1922,54 @@
       <c r="A15" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="H15" s="78"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="M15" s="78"/>
-      <c r="N15" s="78"/>
-      <c r="O15" s="78"/>
-      <c r="P15" s="78"/>
-      <c r="Q15" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="R15" s="78"/>
-      <c r="S15" s="78"/>
-      <c r="T15" s="78"/>
-      <c r="U15" s="78"/>
-      <c r="V15" s="78" t="s">
+      <c r="B15" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="81"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="81"/>
+      <c r="L15" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="M15" s="81"/>
+      <c r="N15" s="81"/>
+      <c r="O15" s="81"/>
+      <c r="P15" s="81"/>
+      <c r="Q15" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="R15" s="81"/>
+      <c r="S15" s="81"/>
+      <c r="T15" s="81"/>
+      <c r="U15" s="81"/>
+      <c r="V15" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="W15" s="78"/>
-      <c r="X15" s="78"/>
-      <c r="Y15" s="78"/>
-      <c r="Z15" s="78"/>
-      <c r="AA15" s="78" t="s">
+      <c r="W15" s="81"/>
+      <c r="X15" s="81"/>
+      <c r="Y15" s="81"/>
+      <c r="Z15" s="81"/>
+      <c r="AA15" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="AB15" s="78"/>
-      <c r="AC15" s="78"/>
-      <c r="AD15" s="78"/>
-      <c r="AE15" s="78"/>
-      <c r="AF15" s="92" t="s">
+      <c r="AB15" s="81"/>
+      <c r="AC15" s="81"/>
+      <c r="AD15" s="81"/>
+      <c r="AE15" s="81"/>
+      <c r="AF15" s="77" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:32" ht="18.95" customHeight="1">
-      <c r="A16" s="78">
+      <c r="A16" s="81">
         <v>4</v>
       </c>
       <c r="B16" s="39">
@@ -2062,10 +2062,10 @@
       <c r="AE16" s="39">
         <v>5</v>
       </c>
-      <c r="AF16" s="92"/>
+      <c r="AF16" s="77"/>
     </row>
     <row r="17" spans="1:32 16383:16383" ht="18.95" customHeight="1">
-      <c r="A17" s="78"/>
+      <c r="A17" s="81"/>
       <c r="B17" s="42"/>
       <c r="C17" s="43"/>
       <c r="D17" s="43"/>
@@ -2103,54 +2103,54 @@
       <c r="A19" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="H19" s="78"/>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
-      <c r="K19" s="78"/>
-      <c r="L19" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="M19" s="78"/>
-      <c r="N19" s="78"/>
-      <c r="O19" s="78"/>
-      <c r="P19" s="78"/>
-      <c r="Q19" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="R19" s="78"/>
-      <c r="S19" s="78"/>
-      <c r="T19" s="78"/>
-      <c r="U19" s="78"/>
-      <c r="V19" s="78" t="s">
+      <c r="B19" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" s="81"/>
+      <c r="N19" s="81"/>
+      <c r="O19" s="81"/>
+      <c r="P19" s="81"/>
+      <c r="Q19" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="R19" s="81"/>
+      <c r="S19" s="81"/>
+      <c r="T19" s="81"/>
+      <c r="U19" s="81"/>
+      <c r="V19" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="W19" s="78"/>
-      <c r="X19" s="78"/>
-      <c r="Y19" s="78"/>
-      <c r="Z19" s="78"/>
-      <c r="AA19" s="78" t="s">
+      <c r="W19" s="81"/>
+      <c r="X19" s="81"/>
+      <c r="Y19" s="81"/>
+      <c r="Z19" s="81"/>
+      <c r="AA19" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="AB19" s="78"/>
-      <c r="AC19" s="78"/>
-      <c r="AD19" s="78"/>
-      <c r="AE19" s="78"/>
-      <c r="AF19" s="92" t="s">
+      <c r="AB19" s="81"/>
+      <c r="AC19" s="81"/>
+      <c r="AD19" s="81"/>
+      <c r="AE19" s="81"/>
+      <c r="AF19" s="77" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:32 16383:16383" ht="18.95" customHeight="1">
-      <c r="A20" s="78">
+      <c r="A20" s="81">
         <v>5</v>
       </c>
       <c r="B20" s="39">
@@ -2243,10 +2243,10 @@
       <c r="AE20" s="39">
         <v>5</v>
       </c>
-      <c r="AF20" s="92"/>
+      <c r="AF20" s="77"/>
     </row>
     <row r="21" spans="1:32 16383:16383" ht="18.95" customHeight="1">
-      <c r="A21" s="78"/>
+      <c r="A21" s="81"/>
       <c r="B21" s="42"/>
       <c r="C21" s="43"/>
       <c r="D21" s="43"/>
@@ -2284,21 +2284,21 @@
       <c r="A23" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="79" t="s">
+      <c r="B23" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="80"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="80"/>
-      <c r="G23" s="81" t="s">
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="82"/>
-      <c r="I23" s="81" t="s">
+      <c r="H23" s="91"/>
+      <c r="I23" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="J23" s="82"/>
+      <c r="J23" s="91"/>
       <c r="L23" s="53" t="s">
         <v>13</v>
       </c>
@@ -2328,19 +2328,19 @@
       <c r="A24" s="73">
         <v>1</v>
       </c>
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="84"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="84"/>
-      <c r="G24" s="85" t="s">
+      <c r="C24" s="83"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="86"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="88"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="86"/>
+      <c r="J24" s="87"/>
       <c r="L24" s="55"/>
       <c r="AF24" s="66"/>
       <c r="XFC24"/>
@@ -2349,19 +2349,19 @@
       <c r="A25" s="73">
         <v>2</v>
       </c>
-      <c r="B25" s="83" t="s">
+      <c r="B25" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="84"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="84"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="85" t="s">
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="83"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="86"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="88"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="86"/>
+      <c r="J25" s="87"/>
       <c r="L25" s="55"/>
       <c r="AF25" s="66"/>
       <c r="XFC25"/>
@@ -2370,19 +2370,19 @@
       <c r="A26" s="73">
         <v>3</v>
       </c>
-      <c r="B26" s="83" t="s">
+      <c r="B26" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="84"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="84"/>
-      <c r="F26" s="84"/>
-      <c r="G26" s="85" t="s">
+      <c r="C26" s="83"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="83"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="H26" s="86"/>
-      <c r="I26" s="87"/>
-      <c r="J26" s="88"/>
+      <c r="H26" s="85"/>
+      <c r="I26" s="86"/>
+      <c r="J26" s="87"/>
       <c r="L26" s="55"/>
       <c r="AF26" s="66"/>
       <c r="XFC26"/>
@@ -2398,35 +2398,35 @@
       <c r="AF27" s="66"/>
     </row>
     <row r="28" spans="1:32 16383:16383" ht="18.95" customHeight="1">
-      <c r="A28" s="89" t="s">
+      <c r="A28" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="89"/>
-      <c r="C28" s="89"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="89"/>
-      <c r="F28" s="89"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="89"/>
-      <c r="I28" s="89"/>
-      <c r="J28" s="89"/>
+      <c r="B28" s="78"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="78"/>
+      <c r="I28" s="78"/>
+      <c r="J28" s="78"/>
       <c r="K28" s="75"/>
       <c r="L28" s="55"/>
       <c r="AF28" s="66"/>
     </row>
     <row r="29" spans="1:32 16383:16383">
-      <c r="A29" s="90" t="s">
+      <c r="A29" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="90"/>
-      <c r="C29" s="90"/>
-      <c r="D29" s="90"/>
-      <c r="E29" s="90"/>
-      <c r="F29" s="90"/>
-      <c r="G29" s="90"/>
-      <c r="H29" s="90"/>
-      <c r="I29" s="90"/>
-      <c r="J29" s="90"/>
+      <c r="B29" s="79"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
       <c r="K29" s="74"/>
       <c r="L29" s="55"/>
       <c r="AF29" s="66"/>
@@ -2474,16 +2474,16 @@
       <c r="AF32" s="66"/>
     </row>
     <row r="33" spans="1:32">
-      <c r="A33" s="91"/>
-      <c r="B33" s="91"/>
-      <c r="C33" s="91"/>
-      <c r="D33" s="91"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="91"/>
-      <c r="G33" s="91"/>
-      <c r="H33" s="91"/>
-      <c r="I33" s="91"/>
-      <c r="J33" s="91"/>
+      <c r="A33" s="80"/>
+      <c r="B33" s="80"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="80"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="80"/>
       <c r="K33" s="74"/>
       <c r="L33" s="60"/>
       <c r="M33" s="59"/>
@@ -2509,11 +2509,30 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="AF7:AF8"/>
-    <mergeCell ref="AF11:AF12"/>
-    <mergeCell ref="AF15:AF16"/>
-    <mergeCell ref="AF19:AF20"/>
-    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="V3:Z3"/>
+    <mergeCell ref="AA3:AE3"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="V7:Z7"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="L11:P11"/>
+    <mergeCell ref="Q11:U11"/>
+    <mergeCell ref="V11:Z11"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="L15:P15"/>
+    <mergeCell ref="Q15:U15"/>
+    <mergeCell ref="V15:Z15"/>
+    <mergeCell ref="AA7:AE7"/>
+    <mergeCell ref="AA11:AE11"/>
     <mergeCell ref="A29:J29"/>
     <mergeCell ref="A33:J33"/>
     <mergeCell ref="A4:A5"/>
@@ -2530,6 +2549,11 @@
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="I23:J23"/>
+    <mergeCell ref="AF7:AF8"/>
+    <mergeCell ref="AF11:AF12"/>
+    <mergeCell ref="AF15:AF16"/>
+    <mergeCell ref="AF19:AF20"/>
+    <mergeCell ref="A28:J28"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="I24:J24"/>
@@ -2541,34 +2565,10 @@
     <mergeCell ref="V19:Z19"/>
     <mergeCell ref="AA19:AE19"/>
     <mergeCell ref="B15:F15"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="L15:P15"/>
-    <mergeCell ref="Q15:U15"/>
-    <mergeCell ref="V15:Z15"/>
-    <mergeCell ref="AA7:AE7"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="L11:P11"/>
-    <mergeCell ref="Q11:U11"/>
-    <mergeCell ref="V11:Z11"/>
-    <mergeCell ref="AA11:AE11"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="V7:Z7"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="V3:Z3"/>
-    <mergeCell ref="AA3:AE3"/>
-    <mergeCell ref="AF3:AF4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="1.18055555555556" right="0.25138888888888899" top="0.25138888888888899" bottom="0.25138888888888899" header="0" footer="0"/>
-  <pageSetup paperSize="5" scale="99" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="10000" scale="99" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2580,7 +2580,7 @@
   <dimension ref="A1:AG40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2593,101 +2593,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="26.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="77"/>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="77"/>
-      <c r="AF1" s="77"/>
-      <c r="AG1" s="77"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="92"/>
+      <c r="AA1" s="92"/>
+      <c r="AB1" s="92"/>
+      <c r="AC1" s="92"/>
+      <c r="AD1" s="92"/>
+      <c r="AE1" s="92"/>
+      <c r="AF1" s="92"/>
+      <c r="AG1" s="92"/>
     </row>
     <row r="2" spans="1:33">
       <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:33">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78"/>
-      <c r="R3" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="S3" s="78"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="78"/>
-      <c r="W3" s="78" t="s">
+      <c r="C3" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
+      <c r="Q3" s="81"/>
+      <c r="R3" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="81"/>
+      <c r="T3" s="81"/>
+      <c r="U3" s="81"/>
+      <c r="V3" s="81"/>
+      <c r="W3" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="78"/>
-      <c r="Z3" s="78"/>
-      <c r="AA3" s="78"/>
-      <c r="AB3" s="78" t="s">
+      <c r="X3" s="81"/>
+      <c r="Y3" s="81"/>
+      <c r="Z3" s="81"/>
+      <c r="AA3" s="81"/>
+      <c r="AB3" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="AC3" s="78"/>
-      <c r="AD3" s="78"/>
-      <c r="AE3" s="78"/>
-      <c r="AF3" s="78"/>
-      <c r="AG3" s="92" t="s">
+      <c r="AC3" s="81"/>
+      <c r="AD3" s="81"/>
+      <c r="AE3" s="81"/>
+      <c r="AF3" s="81"/>
+      <c r="AG3" s="77" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:33">
-      <c r="A4" s="78"/>
-      <c r="B4" s="78"/>
+      <c r="A4" s="81"/>
+      <c r="B4" s="81"/>
       <c r="C4" s="39">
         <v>1</v>
       </c>
@@ -2778,7 +2778,7 @@
       <c r="AF4" s="39">
         <v>5</v>
       </c>
-      <c r="AG4" s="92"/>
+      <c r="AG4" s="77"/>
     </row>
     <row r="5" spans="1:33" ht="18.95" customHeight="1">
       <c r="A5" s="40">
@@ -3195,61 +3195,61 @@
       <c r="AG15" s="64"/>
     </row>
     <row r="16" spans="1:33" ht="18.95" customHeight="1">
-      <c r="A16" s="78" t="s">
+      <c r="A16" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="78" t="s">
+      <c r="B16" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="78"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="78"/>
-      <c r="M16" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="N16" s="78"/>
-      <c r="O16" s="78"/>
-      <c r="P16" s="78"/>
-      <c r="Q16" s="78"/>
-      <c r="R16" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="S16" s="78"/>
-      <c r="T16" s="78"/>
-      <c r="U16" s="78"/>
-      <c r="V16" s="78"/>
-      <c r="W16" s="78" t="s">
+      <c r="C16" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" s="81"/>
+      <c r="O16" s="81"/>
+      <c r="P16" s="81"/>
+      <c r="Q16" s="81"/>
+      <c r="R16" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="S16" s="81"/>
+      <c r="T16" s="81"/>
+      <c r="U16" s="81"/>
+      <c r="V16" s="81"/>
+      <c r="W16" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="X16" s="78"/>
-      <c r="Y16" s="78"/>
-      <c r="Z16" s="78"/>
-      <c r="AA16" s="78"/>
-      <c r="AB16" s="78" t="s">
+      <c r="X16" s="81"/>
+      <c r="Y16" s="81"/>
+      <c r="Z16" s="81"/>
+      <c r="AA16" s="81"/>
+      <c r="AB16" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="AC16" s="78"/>
-      <c r="AD16" s="78"/>
-      <c r="AE16" s="78"/>
-      <c r="AF16" s="78"/>
-      <c r="AG16" s="92" t="s">
+      <c r="AC16" s="81"/>
+      <c r="AD16" s="81"/>
+      <c r="AE16" s="81"/>
+      <c r="AF16" s="81"/>
+      <c r="AG16" s="77" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:33" ht="18.95" customHeight="1">
-      <c r="A17" s="78"/>
-      <c r="B17" s="78"/>
+      <c r="A17" s="81"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="39">
         <v>1</v>
       </c>
@@ -3340,7 +3340,7 @@
       <c r="AF17" s="39">
         <v>5</v>
       </c>
-      <c r="AG17" s="92"/>
+      <c r="AG17" s="77"/>
     </row>
     <row r="18" spans="1:33" ht="18.95" customHeight="1">
       <c r="A18" s="40">
@@ -3757,61 +3757,61 @@
       <c r="AG28" s="64"/>
     </row>
     <row r="29" spans="1:33" ht="18.95" customHeight="1">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="78" t="s">
+      <c r="B29" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="I29" s="78"/>
-      <c r="J29" s="78"/>
-      <c r="K29" s="78"/>
-      <c r="L29" s="78"/>
-      <c r="M29" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="N29" s="78"/>
-      <c r="O29" s="78"/>
-      <c r="P29" s="78"/>
-      <c r="Q29" s="78"/>
-      <c r="R29" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="S29" s="78"/>
-      <c r="T29" s="78"/>
-      <c r="U29" s="78"/>
-      <c r="V29" s="78"/>
-      <c r="W29" s="78" t="s">
+      <c r="C29" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="81"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="81"/>
+      <c r="G29" s="81"/>
+      <c r="H29" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" s="81"/>
+      <c r="J29" s="81"/>
+      <c r="K29" s="81"/>
+      <c r="L29" s="81"/>
+      <c r="M29" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="N29" s="81"/>
+      <c r="O29" s="81"/>
+      <c r="P29" s="81"/>
+      <c r="Q29" s="81"/>
+      <c r="R29" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="S29" s="81"/>
+      <c r="T29" s="81"/>
+      <c r="U29" s="81"/>
+      <c r="V29" s="81"/>
+      <c r="W29" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="X29" s="78"/>
-      <c r="Y29" s="78"/>
-      <c r="Z29" s="78"/>
-      <c r="AA29" s="78"/>
-      <c r="AB29" s="78" t="s">
+      <c r="X29" s="81"/>
+      <c r="Y29" s="81"/>
+      <c r="Z29" s="81"/>
+      <c r="AA29" s="81"/>
+      <c r="AB29" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="AC29" s="78"/>
-      <c r="AD29" s="78"/>
-      <c r="AE29" s="78"/>
-      <c r="AF29" s="78"/>
-      <c r="AG29" s="92" t="s">
+      <c r="AC29" s="81"/>
+      <c r="AD29" s="81"/>
+      <c r="AE29" s="81"/>
+      <c r="AF29" s="81"/>
+      <c r="AG29" s="77" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:33" ht="18.95" customHeight="1">
-      <c r="A30" s="78"/>
-      <c r="B30" s="78"/>
+      <c r="A30" s="81"/>
+      <c r="B30" s="81"/>
       <c r="C30" s="39">
         <v>1</v>
       </c>
@@ -3902,7 +3902,7 @@
       <c r="AF30" s="39">
         <v>5</v>
       </c>
-      <c r="AG30" s="92"/>
+      <c r="AG30" s="77"/>
     </row>
     <row r="31" spans="1:33" ht="18.95" customHeight="1">
       <c r="A31" s="40">
@@ -4285,6 +4285,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="M16:Q16"/>
+    <mergeCell ref="R16:V16"/>
+    <mergeCell ref="W16:AA16"/>
+    <mergeCell ref="A1:AG1"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="R3:V3"/>
+    <mergeCell ref="W3:AA3"/>
+    <mergeCell ref="AB3:AF3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="AG3:AG4"/>
     <mergeCell ref="AG16:AG17"/>
     <mergeCell ref="AG29:AG30"/>
     <mergeCell ref="A16:A17"/>
@@ -4301,22 +4313,10 @@
     <mergeCell ref="AB29:AF29"/>
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="H16:L16"/>
-    <mergeCell ref="M16:Q16"/>
-    <mergeCell ref="R16:V16"/>
-    <mergeCell ref="W16:AA16"/>
-    <mergeCell ref="A1:AG1"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="M3:Q3"/>
-    <mergeCell ref="R3:V3"/>
-    <mergeCell ref="W3:AA3"/>
-    <mergeCell ref="AB3:AF3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="AG3:AG4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="1.18055555555556" right="0.25138888888888899" top="0.25138888888888899" bottom="0.25138888888888899" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="77" orientation="landscape"/>
+  <pageSetup paperSize="10000" scale="78" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4341,101 +4341,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="26.25" customHeight="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="77"/>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="77"/>
-      <c r="AF1" s="77"/>
-      <c r="AG1" s="77"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="92"/>
+      <c r="AA1" s="92"/>
+      <c r="AB1" s="92"/>
+      <c r="AC1" s="92"/>
+      <c r="AD1" s="92"/>
+      <c r="AE1" s="92"/>
+      <c r="AF1" s="92"/>
+      <c r="AG1" s="92"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1">
       <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:33">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78"/>
-      <c r="R3" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="S3" s="78"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="78"/>
-      <c r="W3" s="78" t="s">
+      <c r="C3" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
+      <c r="Q3" s="81"/>
+      <c r="R3" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="81"/>
+      <c r="T3" s="81"/>
+      <c r="U3" s="81"/>
+      <c r="V3" s="81"/>
+      <c r="W3" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="78"/>
-      <c r="Z3" s="78"/>
-      <c r="AA3" s="78"/>
-      <c r="AB3" s="78" t="s">
+      <c r="X3" s="81"/>
+      <c r="Y3" s="81"/>
+      <c r="Z3" s="81"/>
+      <c r="AA3" s="81"/>
+      <c r="AB3" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="AC3" s="78"/>
-      <c r="AD3" s="78"/>
-      <c r="AE3" s="78"/>
-      <c r="AF3" s="78"/>
-      <c r="AG3" s="92" t="s">
+      <c r="AC3" s="81"/>
+      <c r="AD3" s="81"/>
+      <c r="AE3" s="81"/>
+      <c r="AF3" s="81"/>
+      <c r="AG3" s="77" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:33">
-      <c r="A4" s="78"/>
-      <c r="B4" s="78"/>
+      <c r="A4" s="81"/>
+      <c r="B4" s="81"/>
       <c r="C4" s="39">
         <v>1</v>
       </c>
@@ -4526,7 +4526,7 @@
       <c r="AF4" s="39">
         <v>5</v>
       </c>
-      <c r="AG4" s="92"/>
+      <c r="AG4" s="77"/>
     </row>
     <row r="5" spans="1:33" ht="18.95" customHeight="1">
       <c r="A5" s="40">
@@ -4943,61 +4943,61 @@
       <c r="AG15" s="64"/>
     </row>
     <row r="16" spans="1:33" ht="18.95" customHeight="1">
-      <c r="A16" s="78" t="s">
+      <c r="A16" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="78" t="s">
+      <c r="B16" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="78"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="78"/>
-      <c r="M16" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="N16" s="78"/>
-      <c r="O16" s="78"/>
-      <c r="P16" s="78"/>
-      <c r="Q16" s="78"/>
-      <c r="R16" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="S16" s="78"/>
-      <c r="T16" s="78"/>
-      <c r="U16" s="78"/>
-      <c r="V16" s="78"/>
-      <c r="W16" s="78" t="s">
+      <c r="C16" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" s="81"/>
+      <c r="O16" s="81"/>
+      <c r="P16" s="81"/>
+      <c r="Q16" s="81"/>
+      <c r="R16" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="S16" s="81"/>
+      <c r="T16" s="81"/>
+      <c r="U16" s="81"/>
+      <c r="V16" s="81"/>
+      <c r="W16" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="X16" s="78"/>
-      <c r="Y16" s="78"/>
-      <c r="Z16" s="78"/>
-      <c r="AA16" s="78"/>
-      <c r="AB16" s="78" t="s">
+      <c r="X16" s="81"/>
+      <c r="Y16" s="81"/>
+      <c r="Z16" s="81"/>
+      <c r="AA16" s="81"/>
+      <c r="AB16" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="AC16" s="78"/>
-      <c r="AD16" s="78"/>
-      <c r="AE16" s="78"/>
-      <c r="AF16" s="78"/>
-      <c r="AG16" s="92" t="s">
+      <c r="AC16" s="81"/>
+      <c r="AD16" s="81"/>
+      <c r="AE16" s="81"/>
+      <c r="AF16" s="81"/>
+      <c r="AG16" s="77" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:33" ht="18.95" customHeight="1">
-      <c r="A17" s="78"/>
-      <c r="B17" s="78"/>
+      <c r="A17" s="81"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="39">
         <v>1</v>
       </c>
@@ -5088,7 +5088,7 @@
       <c r="AF17" s="39">
         <v>5</v>
       </c>
-      <c r="AG17" s="92"/>
+      <c r="AG17" s="77"/>
     </row>
     <row r="18" spans="1:33" ht="18.95" customHeight="1">
       <c r="A18" s="40">
@@ -5511,14 +5511,14 @@
       <c r="B29" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="81" t="s">
+      <c r="C29" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="82"/>
-      <c r="E29" s="81" t="s">
+      <c r="D29" s="91"/>
+      <c r="E29" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="82"/>
+      <c r="F29" s="91"/>
       <c r="H29" s="53" t="s">
         <v>13</v>
       </c>
@@ -5555,12 +5555,12 @@
       <c r="B30" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="85" t="s">
+      <c r="C30" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="86"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="88"/>
+      <c r="D30" s="85"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="87"/>
       <c r="H30" s="55"/>
       <c r="AG30" s="66"/>
     </row>
@@ -5571,12 +5571,12 @@
       <c r="B31" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="85" t="s">
+      <c r="C31" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="86"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="88"/>
+      <c r="D31" s="85"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="87"/>
       <c r="H31" s="55"/>
       <c r="AG31" s="66"/>
     </row>
@@ -5587,12 +5587,12 @@
       <c r="B32" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="85" t="s">
+      <c r="C32" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="86"/>
-      <c r="E32" s="87"/>
-      <c r="F32" s="88"/>
+      <c r="D32" s="85"/>
+      <c r="E32" s="86"/>
+      <c r="F32" s="87"/>
       <c r="H32" s="55"/>
       <c r="AG32" s="66"/>
     </row>
@@ -5603,12 +5603,12 @@
       <c r="B33" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="85" t="s">
+      <c r="C33" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="86"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="88"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="86"/>
+      <c r="F33" s="87"/>
       <c r="H33" s="55"/>
       <c r="AG33" s="66"/>
     </row>
@@ -5619,12 +5619,12 @@
       <c r="B34" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="85" t="s">
+      <c r="C34" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="86"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="88"/>
+      <c r="D34" s="85"/>
+      <c r="E34" s="86"/>
+      <c r="F34" s="87"/>
       <c r="H34" s="55"/>
       <c r="AG34" s="66"/>
     </row>
@@ -5633,26 +5633,26 @@
       <c r="AG35" s="66"/>
     </row>
     <row r="36" spans="1:33">
-      <c r="A36" s="89" t="s">
+      <c r="A36" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="89"/>
-      <c r="C36" s="89"/>
-      <c r="D36" s="89"/>
-      <c r="E36" s="89"/>
-      <c r="F36" s="89"/>
+      <c r="B36" s="78"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="78"/>
       <c r="H36" s="55"/>
       <c r="AG36" s="66"/>
     </row>
     <row r="37" spans="1:33">
-      <c r="A37" s="90" t="s">
+      <c r="A37" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="90"/>
-      <c r="C37" s="90"/>
-      <c r="D37" s="90"/>
-      <c r="E37" s="90"/>
-      <c r="F37" s="90"/>
+      <c r="B37" s="79"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="79"/>
+      <c r="E37" s="79"/>
+      <c r="F37" s="79"/>
       <c r="H37" s="55"/>
       <c r="AG37" s="66"/>
     </row>
@@ -5684,11 +5684,11 @@
       <c r="AG40" s="66"/>
     </row>
     <row r="41" spans="1:33">
-      <c r="A41" s="93"/>
-      <c r="B41" s="93"/>
-      <c r="C41" s="93"/>
-      <c r="D41" s="93"/>
-      <c r="E41" s="93"/>
+      <c r="A41" s="94"/>
+      <c r="B41" s="94"/>
+      <c r="C41" s="94"/>
+      <c r="D41" s="94"/>
+      <c r="E41" s="94"/>
       <c r="F41" s="59"/>
       <c r="H41" s="60"/>
       <c r="I41" s="59"/>
@@ -5718,11 +5718,30 @@
       <c r="AG41" s="67"/>
     </row>
     <row r="42" spans="1:33">
-      <c r="A42" s="94"/>
-      <c r="B42" s="94"/>
+      <c r="A42" s="93"/>
+      <c r="B42" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A1:AG1"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="R3:V3"/>
+    <mergeCell ref="W3:AA3"/>
+    <mergeCell ref="AB3:AF3"/>
+    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="AB16:AF16"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="M16:Q16"/>
+    <mergeCell ref="R16:V16"/>
+    <mergeCell ref="W16:AA16"/>
     <mergeCell ref="AG16:AG17"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A3:A4"/>
@@ -5739,29 +5758,10 @@
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="AB16:AF16"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="M16:Q16"/>
-    <mergeCell ref="R16:V16"/>
-    <mergeCell ref="W16:AA16"/>
-    <mergeCell ref="A1:AG1"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="M3:Q3"/>
-    <mergeCell ref="R3:V3"/>
-    <mergeCell ref="W3:AA3"/>
-    <mergeCell ref="AB3:AF3"/>
-    <mergeCell ref="AG3:AG4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="1.18055555555556" right="0.25138888888888899" top="0.25138888888888899" bottom="0.25138888888888899" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="78" orientation="landscape"/>
+  <pageSetup paperSize="10000" scale="80" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5782,20 +5782,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
     </row>
     <row r="2" spans="1:12" ht="15.75">
       <c r="A2" s="20"/>
@@ -5812,24 +5812,24 @@
       <c r="L2" s="21"/>
     </row>
     <row r="3" spans="1:12" ht="15.75">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
       <c r="D3" s="23"/>
       <c r="E3" s="22" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="24"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
       <c r="I3" s="24"/>
-      <c r="J3" s="95" t="s">
+      <c r="J3" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
+      <c r="K3" s="106"/>
+      <c r="L3" s="106"/>
     </row>
     <row r="4" spans="1:12" ht="12" customHeight="1">
       <c r="A4" s="20"/>
@@ -5846,27 +5846,27 @@
       <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:12" ht="15.75">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="105" t="s">
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="107"/>
+      <c r="K5" s="107"/>
+      <c r="L5" s="101" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75">
-      <c r="A6" s="100"/>
+      <c r="A6" s="96"/>
       <c r="B6" s="25">
         <v>1</v>
       </c>
@@ -5897,10 +5897,10 @@
       <c r="K6" s="25">
         <v>10</v>
       </c>
-      <c r="L6" s="105"/>
+      <c r="L6" s="101"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="101"/>
+      <c r="A7" s="97"/>
       <c r="B7" s="26"/>
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
@@ -5911,10 +5911,10 @@
       <c r="I7" s="27"/>
       <c r="J7" s="27"/>
       <c r="K7" s="34"/>
-      <c r="L7" s="106"/>
+      <c r="L7" s="102"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="102"/>
+      <c r="A8" s="98"/>
       <c r="B8" s="28"/>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
@@ -5925,10 +5925,10 @@
       <c r="I8" s="29"/>
       <c r="J8" s="29"/>
       <c r="K8" s="35"/>
-      <c r="L8" s="107"/>
+      <c r="L8" s="103"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="101"/>
+      <c r="A9" s="97"/>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
       <c r="D9" s="31"/>
@@ -5939,10 +5939,10 @@
       <c r="I9" s="31"/>
       <c r="J9" s="31"/>
       <c r="K9" s="36"/>
-      <c r="L9" s="106"/>
+      <c r="L9" s="102"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="102"/>
+      <c r="A10" s="98"/>
       <c r="B10" s="28"/>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
@@ -5955,10 +5955,10 @@
       <c r="I10" s="29"/>
       <c r="J10" s="29"/>
       <c r="K10" s="35"/>
-      <c r="L10" s="107"/>
+      <c r="L10" s="103"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="101"/>
+      <c r="A11" s="97"/>
       <c r="B11" s="30"/>
       <c r="C11" s="31"/>
       <c r="D11" s="31"/>
@@ -5969,10 +5969,10 @@
       <c r="I11" s="31"/>
       <c r="J11" s="31"/>
       <c r="K11" s="36"/>
-      <c r="L11" s="106"/>
+      <c r="L11" s="102"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="102"/>
+      <c r="A12" s="98"/>
       <c r="B12" s="28"/>
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
@@ -5983,10 +5983,10 @@
       <c r="I12" s="29"/>
       <c r="J12" s="29"/>
       <c r="K12" s="35"/>
-      <c r="L12" s="107"/>
+      <c r="L12" s="103"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="101"/>
+      <c r="A13" s="97"/>
       <c r="B13" s="30"/>
       <c r="C13" s="31"/>
       <c r="D13" s="31"/>
@@ -5997,10 +5997,10 @@
       <c r="I13" s="31"/>
       <c r="J13" s="31"/>
       <c r="K13" s="36"/>
-      <c r="L13" s="106"/>
+      <c r="L13" s="102"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="102"/>
+      <c r="A14" s="98"/>
       <c r="B14" s="28"/>
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
@@ -6011,10 +6011,10 @@
       <c r="I14" s="29"/>
       <c r="J14" s="29"/>
       <c r="K14" s="35"/>
-      <c r="L14" s="107"/>
+      <c r="L14" s="103"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="101"/>
+      <c r="A15" s="97"/>
       <c r="B15" s="30"/>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
@@ -6025,10 +6025,10 @@
       <c r="I15" s="31"/>
       <c r="J15" s="31"/>
       <c r="K15" s="36"/>
-      <c r="L15" s="106"/>
+      <c r="L15" s="102"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="102"/>
+      <c r="A16" s="98"/>
       <c r="B16" s="28"/>
       <c r="C16" s="29"/>
       <c r="D16" s="29"/>
@@ -6039,133 +6039,133 @@
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="35"/>
-      <c r="L16" s="107"/>
+      <c r="L16" s="103"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="103" t="s">
+      <c r="A18" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="97" t="s">
+      <c r="B18" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="97"/>
-      <c r="D18" s="97"/>
-      <c r="E18" s="97"/>
-      <c r="F18" s="97"/>
-      <c r="G18" s="97"/>
-      <c r="H18" s="97"/>
-      <c r="I18" s="97"/>
-      <c r="J18" s="97"/>
-      <c r="K18" s="97"/>
-      <c r="L18" s="97"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="105"/>
+      <c r="E18" s="105"/>
+      <c r="F18" s="105"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="105"/>
+      <c r="I18" s="105"/>
+      <c r="J18" s="105"/>
+      <c r="K18" s="105"/>
+      <c r="L18" s="105"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="104"/>
-      <c r="B19" s="98" t="s">
+      <c r="A19" s="100"/>
+      <c r="B19" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="98"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="98"/>
-      <c r="F19" s="98" t="s">
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="98"/>
-      <c r="H19" s="98"/>
-      <c r="I19" s="98"/>
-      <c r="J19" s="98" t="s">
+      <c r="G19" s="104"/>
+      <c r="H19" s="104"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="K19" s="98"/>
-      <c r="L19" s="98"/>
+      <c r="K19" s="104"/>
+      <c r="L19" s="104"/>
     </row>
     <row r="20" spans="1:12" ht="33" customHeight="1">
       <c r="A20" s="32"/>
-      <c r="B20" s="98"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="98"/>
-      <c r="F20" s="98"/>
-      <c r="G20" s="98"/>
-      <c r="H20" s="98"/>
-      <c r="I20" s="98"/>
-      <c r="J20" s="98"/>
-      <c r="K20" s="98"/>
-      <c r="L20" s="98"/>
+      <c r="B20" s="104"/>
+      <c r="C20" s="104"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="104"/>
+      <c r="G20" s="104"/>
+      <c r="H20" s="104"/>
+      <c r="I20" s="104"/>
+      <c r="J20" s="104"/>
+      <c r="K20" s="104"/>
+      <c r="L20" s="104"/>
     </row>
     <row r="21" spans="1:12" ht="33" customHeight="1">
       <c r="A21" s="32"/>
-      <c r="B21" s="98"/>
-      <c r="C21" s="98"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="98"/>
-      <c r="F21" s="98"/>
-      <c r="G21" s="98"/>
-      <c r="H21" s="98"/>
-      <c r="I21" s="98"/>
-      <c r="J21" s="98"/>
-      <c r="K21" s="98"/>
-      <c r="L21" s="98"/>
+      <c r="B21" s="104"/>
+      <c r="C21" s="104"/>
+      <c r="D21" s="104"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="104"/>
+      <c r="G21" s="104"/>
+      <c r="H21" s="104"/>
+      <c r="I21" s="104"/>
+      <c r="J21" s="104"/>
+      <c r="K21" s="104"/>
+      <c r="L21" s="104"/>
     </row>
     <row r="22" spans="1:12" ht="33" customHeight="1">
       <c r="A22" s="32"/>
-      <c r="B22" s="98"/>
-      <c r="C22" s="98"/>
-      <c r="D22" s="98"/>
-      <c r="E22" s="98"/>
-      <c r="F22" s="98"/>
-      <c r="G22" s="98"/>
-      <c r="H22" s="98"/>
-      <c r="I22" s="98"/>
-      <c r="J22" s="98"/>
-      <c r="K22" s="98"/>
-      <c r="L22" s="98"/>
+      <c r="B22" s="104"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="104"/>
+      <c r="G22" s="104"/>
+      <c r="H22" s="104"/>
+      <c r="I22" s="104"/>
+      <c r="J22" s="104"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
     </row>
     <row r="23" spans="1:12" ht="33" customHeight="1">
       <c r="A23" s="32"/>
-      <c r="B23" s="98"/>
-      <c r="C23" s="98"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="98"/>
-      <c r="F23" s="98"/>
-      <c r="G23" s="98"/>
-      <c r="H23" s="98"/>
-      <c r="I23" s="98"/>
-      <c r="J23" s="98"/>
-      <c r="K23" s="98"/>
-      <c r="L23" s="98"/>
+      <c r="B23" s="104"/>
+      <c r="C23" s="104"/>
+      <c r="D23" s="104"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="104"/>
+      <c r="G23" s="104"/>
+      <c r="H23" s="104"/>
+      <c r="I23" s="104"/>
+      <c r="J23" s="104"/>
+      <c r="K23" s="104"/>
+      <c r="L23" s="104"/>
     </row>
     <row r="24" spans="1:12" ht="33" customHeight="1">
       <c r="A24" s="32"/>
-      <c r="B24" s="98"/>
-      <c r="C24" s="98"/>
-      <c r="D24" s="98"/>
-      <c r="E24" s="98"/>
-      <c r="F24" s="98"/>
-      <c r="G24" s="98"/>
-      <c r="H24" s="98"/>
-      <c r="I24" s="98"/>
-      <c r="J24" s="98"/>
-      <c r="K24" s="98"/>
-      <c r="L24" s="98"/>
+      <c r="B24" s="104"/>
+      <c r="C24" s="104"/>
+      <c r="D24" s="104"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="104"/>
+      <c r="G24" s="104"/>
+      <c r="H24" s="104"/>
+      <c r="I24" s="104"/>
+      <c r="J24" s="104"/>
+      <c r="K24" s="104"/>
+      <c r="L24" s="104"/>
     </row>
     <row r="26" spans="1:12" ht="15.75">
       <c r="A26" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="K26" s="99" t="s">
+      <c r="K26" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="99"/>
+      <c r="L26" s="95"/>
     </row>
     <row r="27" spans="1:12" ht="15.75">
       <c r="A27" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="K27" s="99" t="s">
+      <c r="K27" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="L27" s="99"/>
+      <c r="L27" s="95"/>
     </row>
     <row r="28" spans="1:12" ht="15.75">
       <c r="A28" s="20" t="s">
@@ -6183,13 +6183,37 @@
       <c r="A30" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="K30" s="99" t="s">
+      <c r="K30" s="95" t="s">
         <v>47</v>
       </c>
-      <c r="L30" s="99"/>
+      <c r="L30" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="B18:L18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="J24:L24"/>
     <mergeCell ref="K26:L26"/>
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="K30:L30"/>
@@ -6206,34 +6230,10 @@
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="L13:L14"/>
     <mergeCell ref="L15:L16"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="B18:L18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="B5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="1.18055555555556" right="0.25138888888888899" top="0.25138888888888899" bottom="0.25138888888888899" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape"/>
+  <pageSetup paperSize="10000" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6244,7 +6244,7 @@
   </sheetPr>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:L19"/>
     </sheetView>
   </sheetViews>
@@ -6256,20 +6256,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="108"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
     </row>
     <row r="2" spans="1:12" ht="15.75">
       <c r="A2" s="2"/>
@@ -6286,26 +6286,26 @@
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="15.75">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="109"/>
-      <c r="C3" s="109"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
       <c r="D3" s="5"/>
       <c r="E3" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="6"/>
-      <c r="G3" s="109" t="s">
+      <c r="G3" s="120" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="109"/>
+      <c r="H3" s="120"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="109" t="s">
+      <c r="J3" s="120" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="109"/>
-      <c r="L3" s="109"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
     </row>
     <row r="4" spans="1:12" ht="12" customHeight="1">
       <c r="A4" s="2"/>
@@ -6322,27 +6322,27 @@
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" ht="15.75">
-      <c r="A5" s="115" t="s">
+      <c r="A5" s="109" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="110" t="s">
+      <c r="B5" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="110"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="110"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="110"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="110"/>
-      <c r="K5" s="110"/>
-      <c r="L5" s="119" t="s">
+      <c r="C5" s="121"/>
+      <c r="D5" s="121"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="121"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="121"/>
+      <c r="K5" s="121"/>
+      <c r="L5" s="114" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75">
-      <c r="A6" s="115"/>
+      <c r="A6" s="109"/>
       <c r="B6" s="7">
         <v>1</v>
       </c>
@@ -6373,10 +6373,10 @@
       <c r="K6" s="7">
         <v>10</v>
       </c>
-      <c r="L6" s="119"/>
+      <c r="L6" s="114"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="116"/>
+      <c r="A7" s="110"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -6387,10 +6387,10 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="16"/>
-      <c r="L7" s="120"/>
+      <c r="L7" s="115"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="117"/>
+      <c r="A8" s="111"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -6401,10 +6401,10 @@
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="17"/>
-      <c r="L8" s="121"/>
+      <c r="L8" s="116"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="116"/>
+      <c r="A9" s="110"/>
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -6415,10 +6415,10 @@
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="18"/>
-      <c r="L9" s="120"/>
+      <c r="L9" s="115"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="117"/>
+      <c r="A10" s="111"/>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -6429,10 +6429,10 @@
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="17"/>
-      <c r="L10" s="121"/>
+      <c r="L10" s="116"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="116"/>
+      <c r="A11" s="110"/>
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -6443,10 +6443,10 @@
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="18"/>
-      <c r="L11" s="120"/>
+      <c r="L11" s="115"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="117"/>
+      <c r="A12" s="111"/>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -6457,10 +6457,10 @@
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="17"/>
-      <c r="L12" s="121"/>
+      <c r="L12" s="116"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="116"/>
+      <c r="A13" s="110"/>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -6471,10 +6471,10 @@
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="K13" s="18"/>
-      <c r="L13" s="120"/>
+      <c r="L13" s="115"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="117"/>
+      <c r="A14" s="111"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -6485,10 +6485,10 @@
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="17"/>
-      <c r="L14" s="121"/>
+      <c r="L14" s="116"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="116"/>
+      <c r="A15" s="110"/>
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -6499,10 +6499,10 @@
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
       <c r="K15" s="18"/>
-      <c r="L15" s="120"/>
+      <c r="L15" s="115"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="117"/>
+      <c r="A16" s="111"/>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -6513,28 +6513,28 @@
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="17"/>
-      <c r="L16" s="121"/>
+      <c r="L16" s="116"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="111" t="s">
+      <c r="B18" s="118" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="111"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="111"/>
-      <c r="F18" s="111"/>
-      <c r="G18" s="111"/>
-      <c r="H18" s="111"/>
-      <c r="I18" s="111"/>
-      <c r="J18" s="111"/>
-      <c r="K18" s="111"/>
-      <c r="L18" s="111"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="118"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="118"/>
+      <c r="L18" s="118"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="118"/>
+      <c r="A19" s="113"/>
       <c r="B19" s="112" t="s">
         <v>39</v>
       </c>
@@ -6555,91 +6555,91 @@
     </row>
     <row r="20" spans="1:12" ht="33" customHeight="1">
       <c r="A20" s="14"/>
-      <c r="B20" s="113"/>
-      <c r="C20" s="113"/>
-      <c r="D20" s="113"/>
-      <c r="E20" s="113"/>
-      <c r="F20" s="113"/>
-      <c r="G20" s="113"/>
-      <c r="H20" s="113"/>
-      <c r="I20" s="113"/>
-      <c r="J20" s="113"/>
-      <c r="K20" s="113"/>
-      <c r="L20" s="113"/>
+      <c r="B20" s="117"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="117"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="117"/>
+      <c r="G20" s="117"/>
+      <c r="H20" s="117"/>
+      <c r="I20" s="117"/>
+      <c r="J20" s="117"/>
+      <c r="K20" s="117"/>
+      <c r="L20" s="117"/>
     </row>
     <row r="21" spans="1:12" ht="33" customHeight="1">
       <c r="A21" s="14"/>
-      <c r="B21" s="113"/>
-      <c r="C21" s="113"/>
-      <c r="D21" s="113"/>
-      <c r="E21" s="113"/>
-      <c r="F21" s="113"/>
-      <c r="G21" s="113"/>
-      <c r="H21" s="113"/>
-      <c r="I21" s="113"/>
-      <c r="J21" s="113"/>
-      <c r="K21" s="113"/>
-      <c r="L21" s="113"/>
+      <c r="B21" s="117"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="117"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="117"/>
+      <c r="G21" s="117"/>
+      <c r="H21" s="117"/>
+      <c r="I21" s="117"/>
+      <c r="J21" s="117"/>
+      <c r="K21" s="117"/>
+      <c r="L21" s="117"/>
     </row>
     <row r="22" spans="1:12" ht="33" customHeight="1">
       <c r="A22" s="14"/>
-      <c r="B22" s="113"/>
-      <c r="C22" s="113"/>
-      <c r="D22" s="113"/>
-      <c r="E22" s="113"/>
-      <c r="F22" s="113"/>
-      <c r="G22" s="113"/>
-      <c r="H22" s="113"/>
-      <c r="I22" s="113"/>
-      <c r="J22" s="113"/>
-      <c r="K22" s="113"/>
-      <c r="L22" s="113"/>
+      <c r="B22" s="117"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="117"/>
+      <c r="E22" s="117"/>
+      <c r="F22" s="117"/>
+      <c r="G22" s="117"/>
+      <c r="H22" s="117"/>
+      <c r="I22" s="117"/>
+      <c r="J22" s="117"/>
+      <c r="K22" s="117"/>
+      <c r="L22" s="117"/>
     </row>
     <row r="23" spans="1:12" ht="33" customHeight="1">
       <c r="A23" s="14"/>
-      <c r="B23" s="113"/>
-      <c r="C23" s="113"/>
-      <c r="D23" s="113"/>
-      <c r="E23" s="113"/>
-      <c r="F23" s="113"/>
-      <c r="G23" s="113"/>
-      <c r="H23" s="113"/>
-      <c r="I23" s="113"/>
-      <c r="J23" s="113"/>
-      <c r="K23" s="113"/>
-      <c r="L23" s="113"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="117"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="117"/>
+      <c r="H23" s="117"/>
+      <c r="I23" s="117"/>
+      <c r="J23" s="117"/>
+      <c r="K23" s="117"/>
+      <c r="L23" s="117"/>
     </row>
     <row r="24" spans="1:12" ht="33" customHeight="1">
       <c r="A24" s="14"/>
-      <c r="B24" s="113"/>
-      <c r="C24" s="113"/>
-      <c r="D24" s="113"/>
-      <c r="E24" s="113"/>
-      <c r="F24" s="113"/>
-      <c r="G24" s="113"/>
-      <c r="H24" s="113"/>
-      <c r="I24" s="113"/>
-      <c r="J24" s="113"/>
-      <c r="K24" s="113"/>
-      <c r="L24" s="113"/>
+      <c r="B24" s="117"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="117"/>
+      <c r="E24" s="117"/>
+      <c r="F24" s="117"/>
+      <c r="G24" s="117"/>
+      <c r="H24" s="117"/>
+      <c r="I24" s="117"/>
+      <c r="J24" s="117"/>
+      <c r="K24" s="117"/>
+      <c r="L24" s="117"/>
     </row>
     <row r="26" spans="1:12" ht="15.75">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K26" s="114" t="s">
+      <c r="K26" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="114"/>
+      <c r="L26" s="108"/>
     </row>
     <row r="27" spans="1:12" ht="15.75">
       <c r="A27" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K27" s="114" t="s">
+      <c r="K27" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="L27" s="114"/>
+      <c r="L27" s="108"/>
     </row>
     <row r="28" spans="1:12" ht="15.75">
       <c r="A28" s="2" t="s">
@@ -6657,13 +6657,37 @@
       <c r="A30" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="K30" s="114" t="s">
+      <c r="K30" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="L30" s="114"/>
+      <c r="L30" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="B18:L18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="J24:L24"/>
     <mergeCell ref="K26:L26"/>
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="K30:L30"/>
@@ -6680,33 +6704,9 @@
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="L13:L14"/>
     <mergeCell ref="L15:L16"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="B18:L18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="B5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="1.18055555555556" right="0.25138888888888899" top="0.25138888888888899" bottom="0.25138888888888899" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape"/>
+  <pageSetup paperSize="10000" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>